<commit_message>
Correction for employee questionnaire done
</commit_message>
<xml_diff>
--- a/Week 5/Questionnaire (Employee).xlsx
+++ b/Week 5/Questionnaire (Employee).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22005"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="645" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D523BF87-B296-406F-AEAB-08294CD50B8E}"/>
+  <xr:revisionPtr revIDLastSave="648" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{38B8D269-EAF7-4281-98D0-9003AAA69310}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="45">
   <si>
     <t>              Perpustakaan Negara Malaysia</t>
   </si>
@@ -43,6 +43,9 @@
     <t>will take around 5 minutes to complete.</t>
   </si>
   <si>
+    <t>General Questions, choose one only</t>
+  </si>
+  <si>
     <t>General Questions</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
   </si>
   <si>
     <t>6. The system often occur error when you use it.</t>
+  </si>
+  <si>
+    <t>About customers, choose one only</t>
   </si>
   <si>
     <t>About customers</t>
@@ -289,26 +295,74 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -318,59 +372,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54:N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="21.75" customHeight="1"/>
@@ -797,130 +803,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="11" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="13">
+      <c r="J4" s="9"/>
+      <c r="K4" s="29">
         <v>43637</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
     </row>
     <row r="6" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:16" ht="21.75" customHeight="1">
       <c r="A7" s="8" t="s">
@@ -985,82 +991,82 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="7" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7" t="s">
+      <c r="J12" s="17"/>
+      <c r="K12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
+      <c r="L12" s="14"/>
+      <c r="M12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="7"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="14"/>
     </row>
     <row r="13" spans="1:16" ht="21.75" customHeight="1">
       <c r="A13" s="8"/>
@@ -1082,7 +1088,7 @@
     </row>
     <row r="14" spans="1:16" ht="21.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1092,7 +1098,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1103,96 +1109,96 @@
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="25" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="18" t="s">
+      <c r="J15" s="22"/>
+      <c r="K15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
     </row>
     <row r="16" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
     </row>
     <row r="17" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
+      <c r="A17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
     </row>
     <row r="18" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+      <c r="A18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
     </row>
     <row r="19" spans="1:16" ht="21.75" customHeight="1">
       <c r="A19" s="2">
@@ -1233,26 +1239,26 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
     </row>
     <row r="21" spans="1:16" ht="21.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1262,7 +1268,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1311,44 +1317,44 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
     </row>
     <row r="24" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A24" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="A24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
     </row>
     <row r="25" spans="1:16" ht="21.75" customHeight="1">
       <c r="A25" s="2">
@@ -1389,44 +1395,44 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
     </row>
     <row r="27" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
+      <c r="A27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
     </row>
     <row r="28" spans="1:16" ht="21.75" customHeight="1">
       <c r="A28" s="2">
@@ -1575,174 +1581,174 @@
       <c r="P34" s="8"/>
     </row>
     <row r="35" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A35" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
+      <c r="A35" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
     </row>
     <row r="36" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A36" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
+      <c r="A36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
     </row>
     <row r="37" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7" t="s">
+      <c r="A37" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="7"/>
-      <c r="M37" s="22" t="s">
+      <c r="D37" s="14"/>
+      <c r="E37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N37" s="23"/>
-      <c r="O37" s="7" t="s">
+      <c r="J37" s="14"/>
+      <c r="K37" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P37" s="7"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N37" s="17"/>
+      <c r="O37" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P37" s="14"/>
     </row>
     <row r="38" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
     </row>
     <row r="39" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A39" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
+      <c r="A39" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
     </row>
     <row r="40" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7" t="s">
+      <c r="A40" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7" t="s">
+      <c r="B40" s="14"/>
+      <c r="C40" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40" s="7"/>
-      <c r="K40" s="22" t="s">
+      <c r="D40" s="14"/>
+      <c r="E40" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="23"/>
-      <c r="M40" s="7" t="s">
+      <c r="J40" s="14"/>
+      <c r="K40" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
     </row>
     <row r="41" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
     </row>
     <row r="42" spans="1:16" ht="21.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1752,7 +1758,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -1763,60 +1769,60 @@
       <c r="P42" s="8"/>
     </row>
     <row r="43" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A43" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20" t="s">
+      <c r="A43" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="20"/>
-      <c r="M43" s="27" t="s">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N43" s="28"/>
-      <c r="O43" s="20" t="s">
+      <c r="J43" s="7"/>
+      <c r="K43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="P43" s="20"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" s="11"/>
+      <c r="O43" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P43" s="7"/>
     </row>
     <row r="44" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
     </row>
     <row r="45" spans="1:16" ht="21.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1826,7 +1832,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -1837,56 +1843,56 @@
       <c r="P45" s="8"/>
     </row>
     <row r="46" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A46" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20" t="s">
+      <c r="A46" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46" s="28"/>
-      <c r="K46" s="20" t="s">
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20" t="s">
+      <c r="J46" s="11"/>
+      <c r="K46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N46" s="20"/>
-      <c r="O46" s="20"/>
-      <c r="P46" s="20"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
     </row>
     <row r="47" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
     </row>
     <row r="48" spans="1:16" ht="21.75" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -1896,7 +1902,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
@@ -1907,86 +1913,86 @@
       <c r="P48" s="8"/>
     </row>
     <row r="49" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="29"/>
-      <c r="P49" s="29"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
     </row>
     <row r="50" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="29"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
     </row>
     <row r="51" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
     </row>
     <row r="52" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A52" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32"/>
+      <c r="A52" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
     </row>
     <row r="53" spans="1:16" ht="21.75" customHeight="1">
       <c r="A53" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -1996,7 +2002,7 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
@@ -2007,42 +2013,42 @@
       <c r="P53" s="8"/>
     </row>
     <row r="54" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A54" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20" t="s">
+      <c r="A54" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H54" s="20"/>
-      <c r="I54" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="J54" s="28"/>
-      <c r="K54" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20" t="s">
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H54" s="7"/>
+      <c r="I54" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N54" s="20"/>
-      <c r="O54" s="20" t="s">
+      <c r="J54" s="11"/>
+      <c r="K54" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P54" s="20"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N54" s="11"/>
+      <c r="O54" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P54" s="7"/>
     </row>
     <row r="56" spans="1:16" ht="21.75" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -2052,7 +2058,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
@@ -2063,125 +2069,77 @@
       <c r="P56" s="8"/>
     </row>
     <row r="57" spans="1:16" ht="21.75" customHeight="1">
-      <c r="A57" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20" t="s">
+      <c r="A57" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J57" s="28"/>
-      <c r="K57" s="20" t="s">
+      <c r="D57" s="7"/>
+      <c r="E57" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20" t="s">
+      <c r="J57" s="11"/>
+      <c r="K57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
-      <c r="P57" s="20"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I7:P7"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="I6:P6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="I8:P8"/>
-    <mergeCell ref="I56:P56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="I53:P53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="I47:P47"/>
-    <mergeCell ref="I48:P48"/>
-    <mergeCell ref="I49:P49"/>
-    <mergeCell ref="I50:P50"/>
-    <mergeCell ref="I52:P52"/>
-    <mergeCell ref="I44:P44"/>
-    <mergeCell ref="I45:P45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="I41:P41"/>
-    <mergeCell ref="I42:P42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="I38:P38"/>
-    <mergeCell ref="I39:P39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="I35:P35"/>
-    <mergeCell ref="I36:P36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="I23:P23"/>
-    <mergeCell ref="I24:P24"/>
-    <mergeCell ref="I26:P26"/>
-    <mergeCell ref="I27:P27"/>
-    <mergeCell ref="I34:P34"/>
-    <mergeCell ref="I16:P16"/>
-    <mergeCell ref="I17:P17"/>
-    <mergeCell ref="I18:P18"/>
-    <mergeCell ref="I20:P20"/>
-    <mergeCell ref="I21:P21"/>
-    <mergeCell ref="I13:P13"/>
-    <mergeCell ref="I14:P14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="I11:P11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="I10:P10"/>
-    <mergeCell ref="I1:P2"/>
-    <mergeCell ref="I3:P3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A42:H42"/>
     <mergeCell ref="A43:B43"/>
@@ -2202,46 +2160,94 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="I10:P10"/>
+    <mergeCell ref="I1:P2"/>
+    <mergeCell ref="I3:P3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I13:P13"/>
+    <mergeCell ref="I14:P14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="I11:P11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="I23:P23"/>
+    <mergeCell ref="I24:P24"/>
+    <mergeCell ref="I26:P26"/>
+    <mergeCell ref="I27:P27"/>
+    <mergeCell ref="I34:P34"/>
+    <mergeCell ref="I16:P16"/>
+    <mergeCell ref="I17:P17"/>
+    <mergeCell ref="I18:P18"/>
+    <mergeCell ref="I20:P20"/>
+    <mergeCell ref="I21:P21"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="I38:P38"/>
+    <mergeCell ref="I39:P39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="I35:P35"/>
+    <mergeCell ref="I36:P36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="I53:P53"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="O54:P54"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I7:P7"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="I6:P6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="I8:P8"/>
+    <mergeCell ref="I56:P56"/>
+    <mergeCell ref="I47:P47"/>
+    <mergeCell ref="I48:P48"/>
+    <mergeCell ref="I49:P49"/>
+    <mergeCell ref="I50:P50"/>
+    <mergeCell ref="I52:P52"/>
+    <mergeCell ref="I44:P44"/>
+    <mergeCell ref="I45:P45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="I41:P41"/>
+    <mergeCell ref="I42:P42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>